<commit_message>
added required elements to IEPD
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/service-specifications/Booking_Reporting_Service/artifacts/service_model/information_model/BookingReport-IEPD/documentation/impl/AdamsCounty/ACSO-DataExports.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/service-specifications/Booking_Reporting_Service/artifacts/service_model/information_model/BookingReport-IEPD/documentation/impl/AdamsCounty/ACSO-DataExports.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26423"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26519"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="26760" yWindow="0" windowWidth="25600" windowHeight="14460"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="46">
   <si>
     <t>Last Name</t>
   </si>
@@ -159,9 +159,6 @@
   </si>
   <si>
     <t>Corizon (Health_Record_Query_Response)</t>
-  </si>
-  <si>
-    <t>Create mapping spreadsheet for the 3 systems, identify which elements come from which system, add ext:SourceSystemNameText along with other ID elements, add photo elements (see LEXS for method)</t>
   </si>
 </sst>
 </file>
@@ -540,7 +537,7 @@
   <dimension ref="A2:P15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="A15" sqref="A15:K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -721,9 +718,7 @@
       </c>
     </row>
     <row r="15" spans="1:16">
-      <c r="A15" s="5" t="s">
-        <v>46</v>
-      </c>
+      <c r="A15" s="5"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>

</xml_diff>